<commit_message>
Weather Scrape Added. Couldn
</commit_message>
<xml_diff>
--- a/Archived_ExcelFile.xlsx
+++ b/Archived_ExcelFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>S.No</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Temperature</t>
   </si>
   <si>
     <t>Capacity</t>
@@ -385,7 +388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,7 +396,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,6 +432,9 @@
       </c>
       <c r="L1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>